<commit_message>
Agregados archivos de DATOS
</commit_message>
<xml_diff>
--- a/superAndes-jdo/data/DATOS.xlsx
+++ b/superAndes-jdo/data/DATOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Inc\Desktop\U\SisTrans\Iteracion 2\sistrans\superAndes-jdo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Inc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74FCE7-80C6-4283-9985-031ADCB664DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{136D9D12-72EE-4452-86C1-9D6CA8DFC2AF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{9796FEAD-349B-4125-A633-D95226379889}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="138">
   <si>
     <t>ID_ALMACENAMIENTO</t>
   </si>
@@ -293,36 +293,6 @@
     <t>Rosas</t>
   </si>
   <si>
-    <t>pedro@me</t>
-  </si>
-  <si>
-    <t>carlos@me</t>
-  </si>
-  <si>
-    <t>fausto@me</t>
-  </si>
-  <si>
-    <t>clira@me</t>
-  </si>
-  <si>
-    <t>feniz@me</t>
-  </si>
-  <si>
-    <t>felix@me</t>
-  </si>
-  <si>
-    <t>abbi@me</t>
-  </si>
-  <si>
-    <t>john@me</t>
-  </si>
-  <si>
-    <t>mhl@me</t>
-  </si>
-  <si>
-    <t>emily@me</t>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
@@ -374,9 +344,6 @@
     <t>POLLO</t>
   </si>
   <si>
-    <t>date '2015-01-01'</t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
@@ -392,9 +359,6 @@
     <t>AJAX</t>
   </si>
   <si>
-    <t>CM3</t>
-  </si>
-  <si>
     <t>REBAJA</t>
   </si>
   <si>
@@ -434,7 +398,52 @@
     <t>SOL</t>
   </si>
   <si>
-    <t>PNATURAL</t>
+    <t>carlos@me.com</t>
+  </si>
+  <si>
+    <t>fausto@me.com</t>
+  </si>
+  <si>
+    <t>clira@me.com</t>
+  </si>
+  <si>
+    <t>feniz@me.com</t>
+  </si>
+  <si>
+    <t>felix@me.com</t>
+  </si>
+  <si>
+    <t>abbi@me.com</t>
+  </si>
+  <si>
+    <t>john@me.com</t>
+  </si>
+  <si>
+    <t>mhl@me.com</t>
+  </si>
+  <si>
+    <t>emily@me.com</t>
+  </si>
+  <si>
+    <t>pedro@me.com</t>
+  </si>
+  <si>
+    <t>HERRAMIENTAS</t>
+  </si>
+  <si>
+    <t>TORNILLO</t>
+  </si>
+  <si>
+    <t>VARIOS</t>
+  </si>
+  <si>
+    <t>VIDEOUEGO</t>
+  </si>
+  <si>
+    <t>Especifico</t>
+  </si>
+  <si>
+    <t>cm3</t>
   </si>
 </sst>
 </file>
@@ -487,10 +496,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -806,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E72C13-854D-4182-ADF2-AE51E01A9708}">
-  <dimension ref="A1:CR11"/>
+  <dimension ref="A1:CR18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0">
-      <selection activeCell="CR2" sqref="CR2:CR11"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BT3" sqref="BT3:BT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,22 +1110,22 @@
         <v>77</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="N2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="O2">
         <v>34</v>
       </c>
       <c r="Q2">
-        <v>123</v>
+        <v>123000000</v>
       </c>
       <c r="R2" t="s">
         <v>69</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="U2">
         <v>1</v>
@@ -1127,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="X2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="Y2">
         <v>23</v>
@@ -1135,8 +1145,8 @@
       <c r="AA2">
         <v>1</v>
       </c>
-      <c r="AB2" t="s">
-        <v>114</v>
+      <c r="AB2" s="3">
+        <v>42005</v>
       </c>
       <c r="AC2">
         <v>1000</v>
@@ -1160,13 +1170,13 @@
         <v>70</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="AL2">
         <v>1</v>
       </c>
       <c r="AM2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="AN2">
         <v>23</v>
@@ -1174,8 +1184,8 @@
       <c r="AP2">
         <v>1</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>77</v>
+      <c r="AQ2">
+        <v>1</v>
       </c>
       <c r="AR2">
         <v>345</v>
@@ -1184,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="AU2">
-        <v>123</v>
+        <v>123000000</v>
       </c>
       <c r="AV2" t="s">
         <v>64</v>
@@ -1196,13 +1206,13 @@
         <v>70</v>
       </c>
       <c r="AY2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>114</v>
+        <v>97</v>
+      </c>
+      <c r="AZ2" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA2" s="3">
+        <v>42005</v>
       </c>
       <c r="BB2">
         <v>1</v>
@@ -1217,13 +1227,13 @@
         <v>1</v>
       </c>
       <c r="BG2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH2">
         <v>1</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="BK2">
         <v>1</v>
@@ -1232,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="BM2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="BN2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="BO2">
         <v>1232</v>
@@ -1253,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="BT2" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU2">
         <v>1232</v>
@@ -1268,43 +1278,43 @@
         <v>1</v>
       </c>
       <c r="BY2">
-        <v>123</v>
+        <v>123000000</v>
       </c>
       <c r="CA2">
         <v>1</v>
       </c>
       <c r="CB2">
-        <v>123</v>
+        <v>123000000</v>
       </c>
       <c r="CC2" t="s">
         <v>22</v>
       </c>
       <c r="CD2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="CE2">
         <v>1</v>
       </c>
-      <c r="CF2" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>114</v>
+      <c r="CF2" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG2" s="3">
+        <v>42005</v>
       </c>
       <c r="CH2">
         <v>1</v>
       </c>
       <c r="CJ2">
-        <v>123</v>
+        <v>123000000</v>
       </c>
       <c r="CK2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="CL2">
         <v>1</v>
       </c>
       <c r="CM2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO2" t="s">
         <v>64</v>
@@ -1351,22 +1361,22 @@
         <v>78</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="N3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="O3">
         <v>5</v>
       </c>
       <c r="Q3">
-        <v>456</v>
+        <v>456000000</v>
       </c>
       <c r="R3" t="s">
         <v>73</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -1378,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="X3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="Y3">
         <v>44</v>
@@ -1386,8 +1396,8 @@
       <c r="AA3">
         <v>2</v>
       </c>
-      <c r="AB3" t="s">
-        <v>114</v>
+      <c r="AB3" s="3">
+        <v>42005</v>
       </c>
       <c r="AC3">
         <v>2344</v>
@@ -1411,13 +1421,13 @@
         <v>74</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="AL3">
         <v>2</v>
       </c>
       <c r="AM3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="AN3">
         <v>44</v>
@@ -1425,8 +1435,8 @@
       <c r="AP3">
         <v>2</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>78</v>
+      <c r="AQ3">
+        <v>2</v>
       </c>
       <c r="AR3">
         <v>555</v>
@@ -1435,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="AU3">
-        <v>456</v>
+        <v>456000000</v>
       </c>
       <c r="AV3" t="s">
         <v>65</v>
@@ -1447,13 +1457,13 @@
         <v>74</v>
       </c>
       <c r="AY3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="AZ3" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA3" s="3">
+        <v>42005</v>
       </c>
       <c r="BB3">
         <v>2</v>
@@ -1468,13 +1478,13 @@
         <v>2</v>
       </c>
       <c r="BG3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH3">
         <v>2</v>
       </c>
       <c r="BI3" s="1" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="BK3">
         <v>2</v>
@@ -1483,10 +1493,10 @@
         <v>2</v>
       </c>
       <c r="BM3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="BN3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="BO3">
         <v>222</v>
@@ -1504,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="BT3" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU3">
         <v>222</v>
@@ -1519,43 +1529,43 @@
         <v>2</v>
       </c>
       <c r="BY3">
-        <v>456</v>
+        <v>456000000</v>
       </c>
       <c r="CA3">
         <v>2</v>
       </c>
       <c r="CB3">
-        <v>456</v>
+        <v>456000000</v>
       </c>
       <c r="CC3" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="CD3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CE3">
         <v>2</v>
       </c>
-      <c r="CF3" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>114</v>
+      <c r="CF3" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG3" s="3">
+        <v>42005</v>
       </c>
       <c r="CH3" s="2">
         <v>1</v>
       </c>
       <c r="CJ3">
-        <v>456</v>
+        <v>456000000</v>
       </c>
       <c r="CK3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="CL3">
         <v>2</v>
       </c>
       <c r="CM3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO3" t="s">
         <v>65</v>
@@ -1602,22 +1612,22 @@
         <v>79</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="N4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="O4">
         <v>6</v>
       </c>
       <c r="Q4">
-        <v>789</v>
+        <v>789000000</v>
       </c>
       <c r="R4" t="s">
         <v>71</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="U4">
         <v>3</v>
@@ -1629,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="Y4">
         <v>5</v>
@@ -1637,8 +1647,8 @@
       <c r="AA4">
         <v>3</v>
       </c>
-      <c r="AB4" t="s">
-        <v>114</v>
+      <c r="AB4" s="3">
+        <v>42005</v>
       </c>
       <c r="AC4">
         <v>20000</v>
@@ -1662,13 +1672,13 @@
         <v>72</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="AL4">
         <v>3</v>
       </c>
       <c r="AM4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AN4">
         <v>5</v>
@@ -1676,8 +1686,8 @@
       <c r="AP4">
         <v>3</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>79</v>
+      <c r="AQ4">
+        <v>3</v>
       </c>
       <c r="AR4">
         <v>22</v>
@@ -1686,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="AU4">
-        <v>789</v>
+        <v>789000000</v>
       </c>
       <c r="AV4" t="s">
         <v>66</v>
@@ -1698,13 +1708,13 @@
         <v>72</v>
       </c>
       <c r="AY4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>114</v>
+        <v>99</v>
+      </c>
+      <c r="AZ4" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA4" s="3">
+        <v>42005</v>
       </c>
       <c r="BB4">
         <v>3</v>
@@ -1719,13 +1729,13 @@
         <v>3</v>
       </c>
       <c r="BG4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH4">
         <v>3</v>
       </c>
       <c r="BI4" s="1" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="BK4">
         <v>3</v>
@@ -1734,10 +1744,10 @@
         <v>3</v>
       </c>
       <c r="BM4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="BN4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="BO4">
         <v>34000</v>
@@ -1755,7 +1765,7 @@
         <v>1</v>
       </c>
       <c r="BT4" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU4">
         <v>34000</v>
@@ -1770,43 +1780,43 @@
         <v>3</v>
       </c>
       <c r="BY4">
-        <v>789</v>
+        <v>789000000</v>
       </c>
       <c r="CA4">
         <v>3</v>
       </c>
       <c r="CB4">
-        <v>789</v>
+        <v>789000000</v>
       </c>
       <c r="CC4" t="s">
         <v>22</v>
       </c>
       <c r="CD4" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="CE4">
         <v>3</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CF4" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG4" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CJ4">
+        <v>789000000</v>
+      </c>
+      <c r="CK4" t="s">
         <v>114</v>
-      </c>
-      <c r="CG4" t="s">
-        <v>114</v>
-      </c>
-      <c r="CH4" s="2">
-        <v>1</v>
-      </c>
-      <c r="CJ4">
-        <v>789</v>
-      </c>
-      <c r="CK4" t="s">
-        <v>126</v>
       </c>
       <c r="CL4">
         <v>3</v>
       </c>
       <c r="CM4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO4" t="s">
         <v>66</v>
@@ -1853,34 +1863,34 @@
         <v>80</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="N5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="O5">
         <v>21</v>
       </c>
       <c r="Q5">
-        <v>890</v>
+        <v>890000000</v>
       </c>
       <c r="R5" t="s">
         <v>71</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="U5">
         <v>4</v>
       </c>
       <c r="V5" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="W5">
         <v>3</v>
       </c>
       <c r="X5" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="Y5">
         <v>33</v>
@@ -1888,8 +1898,8 @@
       <c r="AA5">
         <v>4</v>
       </c>
-      <c r="AB5" t="s">
-        <v>114</v>
+      <c r="AB5" s="3">
+        <v>42005</v>
       </c>
       <c r="AC5">
         <v>2000</v>
@@ -1913,13 +1923,13 @@
         <v>72</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="AL5">
         <v>4</v>
       </c>
       <c r="AM5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="AN5">
         <v>33</v>
@@ -1927,8 +1937,8 @@
       <c r="AP5">
         <v>4</v>
       </c>
-      <c r="AQ5" t="s">
-        <v>80</v>
+      <c r="AQ5">
+        <v>4</v>
       </c>
       <c r="AR5">
         <v>1</v>
@@ -1937,7 +1947,7 @@
         <v>4</v>
       </c>
       <c r="AU5">
-        <v>890</v>
+        <v>890000000</v>
       </c>
       <c r="AV5" t="s">
         <v>66</v>
@@ -1949,13 +1959,13 @@
         <v>72</v>
       </c>
       <c r="AY5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>114</v>
+        <v>97</v>
+      </c>
+      <c r="AZ5" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA5" s="3">
+        <v>42005</v>
       </c>
       <c r="BB5">
         <v>4</v>
@@ -1970,13 +1980,13 @@
         <v>55</v>
       </c>
       <c r="BG5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH5">
         <v>4</v>
       </c>
       <c r="BI5" s="1" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="BK5">
         <v>4</v>
@@ -1985,10 +1995,10 @@
         <v>4</v>
       </c>
       <c r="BM5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="BN5" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="BO5">
         <v>1200</v>
@@ -2006,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="BT5" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU5">
         <v>1200</v>
@@ -2021,43 +2031,43 @@
         <v>4</v>
       </c>
       <c r="BY5">
-        <v>890</v>
+        <v>890000000</v>
       </c>
       <c r="CA5">
         <v>4</v>
       </c>
       <c r="CB5">
-        <v>890</v>
+        <v>890000000</v>
       </c>
       <c r="CC5" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="CD5" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CE5">
         <v>4</v>
       </c>
-      <c r="CF5" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG5" t="s">
-        <v>114</v>
+      <c r="CF5" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG5" s="3">
+        <v>42005</v>
       </c>
       <c r="CH5" s="2">
         <v>1</v>
       </c>
       <c r="CJ5">
-        <v>890</v>
+        <v>890000000</v>
       </c>
       <c r="CK5" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="CL5">
         <v>4</v>
       </c>
       <c r="CM5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO5" t="s">
         <v>66</v>
@@ -2104,34 +2114,34 @@
         <v>81</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="N6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="O6">
         <v>44</v>
       </c>
       <c r="Q6">
-        <v>234</v>
+        <v>234000000</v>
       </c>
       <c r="R6" t="s">
         <v>73</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="U6">
         <v>5</v>
       </c>
       <c r="V6" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="W6">
         <v>9</v>
       </c>
       <c r="X6" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="Y6">
         <v>3</v>
@@ -2139,8 +2149,8 @@
       <c r="AA6">
         <v>5</v>
       </c>
-      <c r="AB6" t="s">
-        <v>114</v>
+      <c r="AB6" s="3">
+        <v>42005</v>
       </c>
       <c r="AC6">
         <v>4300</v>
@@ -2164,13 +2174,13 @@
         <v>74</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="AL6">
         <v>5</v>
       </c>
       <c r="AM6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="AN6">
         <v>3</v>
@@ -2178,8 +2188,8 @@
       <c r="AP6">
         <v>5</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>81</v>
+      <c r="AQ6">
+        <v>5</v>
       </c>
       <c r="AR6">
         <v>1</v>
@@ -2188,7 +2198,7 @@
         <v>5</v>
       </c>
       <c r="AU6">
-        <v>234</v>
+        <v>234000000</v>
       </c>
       <c r="AV6" t="s">
         <v>65</v>
@@ -2200,13 +2210,13 @@
         <v>74</v>
       </c>
       <c r="AY6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>114</v>
+        <v>97</v>
+      </c>
+      <c r="AZ6" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA6" s="3">
+        <v>42005</v>
       </c>
       <c r="BB6">
         <v>5</v>
@@ -2221,13 +2231,13 @@
         <v>4</v>
       </c>
       <c r="BG6" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH6">
         <v>5</v>
       </c>
       <c r="BI6" s="1" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="BK6">
         <v>5</v>
@@ -2236,10 +2246,10 @@
         <v>5</v>
       </c>
       <c r="BM6" t="s">
+        <v>97</v>
+      </c>
+      <c r="BN6" t="s">
         <v>107</v>
-      </c>
-      <c r="BN6" t="s">
-        <v>118</v>
       </c>
       <c r="BO6">
         <v>22000</v>
@@ -2257,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="BT6" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU6">
         <v>22000</v>
@@ -2272,43 +2282,43 @@
         <v>5</v>
       </c>
       <c r="BY6">
-        <v>234</v>
+        <v>234000000</v>
       </c>
       <c r="CA6">
         <v>5</v>
       </c>
       <c r="CB6">
-        <v>234</v>
+        <v>234000000</v>
       </c>
       <c r="CC6" t="s">
         <v>22</v>
       </c>
       <c r="CD6" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="CE6">
         <v>5</v>
       </c>
-      <c r="CF6" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG6" t="s">
-        <v>114</v>
+      <c r="CF6" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG6" s="3">
+        <v>42005</v>
       </c>
       <c r="CH6" s="2">
         <v>1</v>
       </c>
       <c r="CJ6">
-        <v>234</v>
+        <v>234000000</v>
       </c>
       <c r="CK6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="CL6">
         <v>5</v>
       </c>
       <c r="CM6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO6" t="s">
         <v>65</v>
@@ -2355,22 +2365,22 @@
         <v>82</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="N7" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="O7">
         <v>55</v>
       </c>
       <c r="Q7">
-        <v>457</v>
+        <v>457000000</v>
       </c>
       <c r="R7" t="s">
         <v>69</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="U7">
         <v>6</v>
@@ -2382,7 +2392,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Y7">
         <v>11</v>
@@ -2390,8 +2400,8 @@
       <c r="AA7">
         <v>6</v>
       </c>
-      <c r="AB7" t="s">
-        <v>114</v>
+      <c r="AB7" s="3">
+        <v>42005</v>
       </c>
       <c r="AC7">
         <v>2200</v>
@@ -2415,13 +2425,13 @@
         <v>70</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="AL7">
         <v>6</v>
       </c>
       <c r="AM7" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AN7">
         <v>11</v>
@@ -2429,8 +2439,8 @@
       <c r="AP7">
         <v>6</v>
       </c>
-      <c r="AQ7" t="s">
-        <v>82</v>
+      <c r="AQ7">
+        <v>6</v>
       </c>
       <c r="AR7">
         <v>22</v>
@@ -2439,7 +2449,7 @@
         <v>6</v>
       </c>
       <c r="AU7">
-        <v>457</v>
+        <v>457000000</v>
       </c>
       <c r="AV7" t="s">
         <v>64</v>
@@ -2451,13 +2461,13 @@
         <v>70</v>
       </c>
       <c r="AY7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>114</v>
+        <v>100</v>
+      </c>
+      <c r="AZ7" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA7" s="3">
+        <v>42005</v>
       </c>
       <c r="BB7">
         <v>6</v>
@@ -2472,13 +2482,13 @@
         <v>6</v>
       </c>
       <c r="BG7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH7">
         <v>6</v>
       </c>
       <c r="BI7" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="BK7">
         <v>6</v>
@@ -2487,10 +2497,10 @@
         <v>6</v>
       </c>
       <c r="BM7" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="BN7" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="BO7">
         <v>2300</v>
@@ -2508,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="BT7" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU7">
         <v>2300</v>
@@ -2523,43 +2533,43 @@
         <v>6</v>
       </c>
       <c r="BY7">
-        <v>457</v>
+        <v>457000000</v>
       </c>
       <c r="CA7">
         <v>6</v>
       </c>
       <c r="CB7">
-        <v>457</v>
+        <v>457000000</v>
       </c>
       <c r="CC7" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="CD7" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CE7">
         <v>6</v>
       </c>
-      <c r="CF7" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG7" t="s">
-        <v>114</v>
+      <c r="CF7" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG7" s="3">
+        <v>42005</v>
       </c>
       <c r="CH7" s="2">
         <v>1</v>
       </c>
       <c r="CJ7">
-        <v>457</v>
+        <v>457000000</v>
       </c>
       <c r="CK7" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="CL7">
         <v>6</v>
       </c>
       <c r="CM7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO7" t="s">
         <v>64</v>
@@ -2606,43 +2616,28 @@
         <v>83</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="N8" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="O8">
         <v>66</v>
       </c>
       <c r="Q8">
-        <v>321</v>
+        <v>321000000</v>
       </c>
       <c r="R8" t="s">
         <v>75</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="U8">
-        <v>7</v>
-      </c>
-      <c r="V8" t="s">
-        <v>62</v>
-      </c>
-      <c r="W8">
-        <v>7</v>
-      </c>
-      <c r="X8" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y8">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="AA8">
         <v>7</v>
       </c>
-      <c r="AB8" t="s">
-        <v>114</v>
+      <c r="AB8" s="3">
+        <v>42005</v>
       </c>
       <c r="AC8">
         <v>399</v>
@@ -2666,13 +2661,13 @@
         <v>72</v>
       </c>
       <c r="AJ8" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="AL8">
         <v>7</v>
       </c>
       <c r="AM8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AN8">
         <v>23</v>
@@ -2680,8 +2675,8 @@
       <c r="AP8">
         <v>7</v>
       </c>
-      <c r="AQ8" t="s">
-        <v>83</v>
+      <c r="AQ8">
+        <v>7</v>
       </c>
       <c r="AR8">
         <v>4444</v>
@@ -2690,7 +2685,7 @@
         <v>7</v>
       </c>
       <c r="AU8">
-        <v>321</v>
+        <v>321000000</v>
       </c>
       <c r="AV8" t="s">
         <v>67</v>
@@ -2702,13 +2697,13 @@
         <v>72</v>
       </c>
       <c r="AY8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA8" t="s">
-        <v>114</v>
+        <v>100</v>
+      </c>
+      <c r="AZ8" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA8" s="3">
+        <v>42005</v>
       </c>
       <c r="BB8">
         <v>7</v>
@@ -2723,13 +2718,13 @@
         <v>77</v>
       </c>
       <c r="BG8" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH8">
         <v>7</v>
       </c>
       <c r="BI8" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="BK8">
         <v>7</v>
@@ -2738,10 +2733,10 @@
         <v>7</v>
       </c>
       <c r="BM8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="BN8" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="BO8">
         <v>2000</v>
@@ -2759,7 +2754,7 @@
         <v>1</v>
       </c>
       <c r="BT8" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU8">
         <v>2000</v>
@@ -2774,43 +2769,43 @@
         <v>7</v>
       </c>
       <c r="BY8">
-        <v>321</v>
+        <v>321000000</v>
       </c>
       <c r="CA8">
         <v>7</v>
       </c>
       <c r="CB8">
-        <v>321</v>
+        <v>321000000</v>
       </c>
       <c r="CC8" t="s">
         <v>22</v>
       </c>
       <c r="CD8" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="CE8">
         <v>7</v>
       </c>
-      <c r="CF8" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG8" t="s">
-        <v>114</v>
+      <c r="CF8" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG8" s="3">
+        <v>42005</v>
       </c>
       <c r="CH8" s="2">
         <v>1</v>
       </c>
       <c r="CJ8">
-        <v>321</v>
+        <v>321000000</v>
       </c>
       <c r="CK8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="CL8">
         <v>7</v>
       </c>
       <c r="CM8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO8" t="s">
         <v>67</v>
@@ -2857,43 +2852,28 @@
         <v>84</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="N9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="O9">
         <v>88</v>
       </c>
       <c r="Q9">
-        <v>432</v>
+        <v>432000000</v>
       </c>
       <c r="R9" t="s">
         <v>76</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="U9">
-        <v>8</v>
-      </c>
-      <c r="V9" t="s">
-        <v>61</v>
-      </c>
-      <c r="W9">
-        <v>6</v>
-      </c>
-      <c r="X9" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y9">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="AA9">
         <v>8</v>
       </c>
-      <c r="AB9" t="s">
-        <v>114</v>
+      <c r="AB9" s="3">
+        <v>42005</v>
       </c>
       <c r="AC9">
         <v>999</v>
@@ -2901,6 +2881,9 @@
       <c r="AD9">
         <v>44</v>
       </c>
+      <c r="AE9">
+        <v>2</v>
+      </c>
       <c r="AF9">
         <v>1</v>
       </c>
@@ -2914,13 +2897,13 @@
         <v>72</v>
       </c>
       <c r="AJ9" s="1" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="AL9">
         <v>8</v>
       </c>
       <c r="AM9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="AN9">
         <v>4</v>
@@ -2928,8 +2911,8 @@
       <c r="AP9">
         <v>8</v>
       </c>
-      <c r="AQ9" t="s">
-        <v>84</v>
+      <c r="AQ9">
+        <v>8</v>
       </c>
       <c r="AR9">
         <v>667</v>
@@ -2938,7 +2921,7 @@
         <v>8</v>
       </c>
       <c r="AU9">
-        <v>432</v>
+        <v>432000000</v>
       </c>
       <c r="AV9" t="s">
         <v>68</v>
@@ -2950,13 +2933,13 @@
         <v>72</v>
       </c>
       <c r="AY9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA9" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA9" s="3">
+        <v>42005</v>
       </c>
       <c r="BB9">
         <v>8</v>
@@ -2971,13 +2954,13 @@
         <v>44</v>
       </c>
       <c r="BG9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH9">
         <v>8</v>
       </c>
       <c r="BI9" s="1" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="BK9">
         <v>8</v>
@@ -2986,10 +2969,10 @@
         <v>8</v>
       </c>
       <c r="BM9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="BN9" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="BO9">
         <v>20000</v>
@@ -3007,7 +2990,7 @@
         <v>1</v>
       </c>
       <c r="BT9" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU9">
         <v>20000</v>
@@ -3022,43 +3005,43 @@
         <v>8</v>
       </c>
       <c r="BY9">
-        <v>432</v>
+        <v>432000000</v>
       </c>
       <c r="CA9">
         <v>8</v>
       </c>
       <c r="CB9">
-        <v>432</v>
+        <v>432000000</v>
       </c>
       <c r="CC9" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="CD9" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CE9">
         <v>8</v>
       </c>
-      <c r="CF9" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG9" t="s">
-        <v>114</v>
+      <c r="CF9" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG9" s="3">
+        <v>42005</v>
       </c>
       <c r="CH9" s="2">
         <v>1</v>
       </c>
       <c r="CJ9">
-        <v>432</v>
+        <v>432000000</v>
       </c>
       <c r="CK9" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="CL9">
         <v>8</v>
       </c>
       <c r="CM9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="CO9" t="s">
         <v>68</v>
@@ -3105,43 +3088,28 @@
         <v>85</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="N10" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O10">
         <v>99</v>
       </c>
       <c r="Q10">
-        <v>978</v>
+        <v>978000000</v>
       </c>
       <c r="R10" t="s">
         <v>76</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="U10">
-        <v>9</v>
-      </c>
-      <c r="V10" t="s">
-        <v>60</v>
-      </c>
-      <c r="W10">
-        <v>5</v>
-      </c>
-      <c r="X10" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y10">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="AA10">
         <v>9</v>
       </c>
-      <c r="AB10" t="s">
-        <v>114</v>
+      <c r="AB10" s="3">
+        <v>42005</v>
       </c>
       <c r="AC10">
         <v>111</v>
@@ -3165,13 +3133,13 @@
         <v>72</v>
       </c>
       <c r="AJ10" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="AL10">
         <v>9</v>
       </c>
       <c r="AM10" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="AN10">
         <v>7</v>
@@ -3179,8 +3147,8 @@
       <c r="AP10">
         <v>9</v>
       </c>
-      <c r="AQ10" t="s">
-        <v>85</v>
+      <c r="AQ10">
+        <v>9</v>
       </c>
       <c r="AR10">
         <v>7664</v>
@@ -3189,7 +3157,7 @@
         <v>9</v>
       </c>
       <c r="AU10">
-        <v>978</v>
+        <v>978000000</v>
       </c>
       <c r="AV10" t="s">
         <v>68</v>
@@ -3201,13 +3169,13 @@
         <v>72</v>
       </c>
       <c r="AY10" t="s">
-        <v>112</v>
-      </c>
-      <c r="AZ10" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA10" t="s">
-        <v>114</v>
+        <v>102</v>
+      </c>
+      <c r="AZ10" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA10" s="3">
+        <v>42005</v>
       </c>
       <c r="BB10">
         <v>9</v>
@@ -3222,13 +3190,13 @@
         <v>22</v>
       </c>
       <c r="BG10" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH10">
         <v>9</v>
       </c>
       <c r="BI10" s="1" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="BK10">
         <v>9</v>
@@ -3237,10 +3205,10 @@
         <v>9</v>
       </c>
       <c r="BM10" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="BN10" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="BO10">
         <v>2000</v>
@@ -3258,7 +3226,7 @@
         <v>1</v>
       </c>
       <c r="BT10" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU10">
         <v>2000</v>
@@ -3273,55 +3241,43 @@
         <v>9</v>
       </c>
       <c r="BY10">
-        <v>978</v>
+        <v>978000000</v>
       </c>
       <c r="CA10">
         <v>9</v>
       </c>
       <c r="CB10">
-        <v>978</v>
+        <v>978000000</v>
       </c>
       <c r="CC10" t="s">
         <v>22</v>
       </c>
       <c r="CD10" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="CE10">
         <v>9</v>
       </c>
-      <c r="CF10" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG10" t="s">
-        <v>114</v>
+      <c r="CF10" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG10" s="3">
+        <v>42005</v>
       </c>
       <c r="CH10" s="2">
         <v>1</v>
       </c>
       <c r="CJ10">
-        <v>978</v>
+        <v>978000000</v>
       </c>
       <c r="CK10" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="CL10">
         <v>9</v>
       </c>
       <c r="CM10" t="s">
-        <v>134</v>
-      </c>
-      <c r="CO10" t="s">
-        <v>68</v>
-      </c>
-      <c r="CP10" t="s">
-        <v>76</v>
-      </c>
-      <c r="CQ10" t="s">
-        <v>72</v>
-      </c>
-      <c r="CR10">
-        <v>9</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.25">
@@ -3356,43 +3312,28 @@
         <v>86</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="N11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="O11">
         <v>12</v>
       </c>
       <c r="Q11">
-        <v>222</v>
+        <v>222000000</v>
       </c>
       <c r="R11" t="s">
         <v>75</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="U11">
-        <v>10</v>
-      </c>
-      <c r="V11" t="s">
-        <v>63</v>
-      </c>
-      <c r="W11">
-        <v>2</v>
-      </c>
-      <c r="X11" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y11">
-        <v>8</v>
+        <v>131</v>
       </c>
       <c r="AA11">
         <v>10</v>
       </c>
-      <c r="AB11" t="s">
-        <v>114</v>
+      <c r="AB11" s="3">
+        <v>42005</v>
       </c>
       <c r="AC11">
         <v>345</v>
@@ -3416,13 +3357,13 @@
         <v>72</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="AL11">
         <v>10</v>
       </c>
       <c r="AM11" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="AN11">
         <v>8</v>
@@ -3430,14 +3371,14 @@
       <c r="AP11">
         <v>10</v>
       </c>
-      <c r="AQ11" t="s">
-        <v>86</v>
+      <c r="AQ11">
+        <v>10</v>
       </c>
       <c r="AT11">
         <v>10</v>
       </c>
       <c r="AU11">
-        <v>222</v>
+        <v>222000000</v>
       </c>
       <c r="AV11" t="s">
         <v>67</v>
@@ -3449,13 +3390,13 @@
         <v>72</v>
       </c>
       <c r="AY11" t="s">
-        <v>113</v>
-      </c>
-      <c r="AZ11" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA11" t="s">
-        <v>114</v>
+        <v>103</v>
+      </c>
+      <c r="AZ11" s="3">
+        <v>42005</v>
+      </c>
+      <c r="BA11" s="3">
+        <v>42005</v>
       </c>
       <c r="BB11">
         <v>10</v>
@@ -3470,13 +3411,13 @@
         <v>33</v>
       </c>
       <c r="BG11" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="BH11">
         <v>10</v>
       </c>
       <c r="BI11" s="1" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="BK11">
         <v>10</v>
@@ -3485,10 +3426,10 @@
         <v>10</v>
       </c>
       <c r="BM11" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="BN11" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="BO11">
         <v>20000</v>
@@ -3506,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="BT11" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="BU11">
         <v>20000</v>
@@ -3521,56 +3462,47 @@
         <v>10</v>
       </c>
       <c r="BY11">
-        <v>222</v>
+        <v>222000000</v>
       </c>
       <c r="CA11">
         <v>10</v>
       </c>
       <c r="CB11">
-        <v>222</v>
+        <v>222000000</v>
       </c>
       <c r="CC11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="CD11" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="CE11">
         <v>10</v>
       </c>
-      <c r="CF11" t="s">
-        <v>114</v>
-      </c>
-      <c r="CG11" t="s">
-        <v>114</v>
+      <c r="CF11" s="3">
+        <v>42005</v>
+      </c>
+      <c r="CG11" s="3">
+        <v>42005</v>
       </c>
       <c r="CH11" s="2">
         <v>1</v>
       </c>
       <c r="CJ11">
-        <v>222</v>
+        <v>222000000</v>
       </c>
       <c r="CK11" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="CL11">
         <v>10</v>
       </c>
       <c r="CM11" t="s">
-        <v>134</v>
-      </c>
-      <c r="CO11" t="s">
-        <v>67</v>
-      </c>
-      <c r="CP11" t="s">
-        <v>75</v>
-      </c>
-      <c r="CQ11" t="s">
-        <v>72</v>
-      </c>
-      <c r="CR11">
-        <v>10</v>
-      </c>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q18" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3583,35 +3515,39 @@
     <hyperlink ref="M8" r:id="rId7" xr:uid="{50EFDF4B-A248-40A5-A8EA-E9D965497971}"/>
     <hyperlink ref="M9" r:id="rId8" xr:uid="{92D0C852-2F2F-45E9-9A14-10346F8C20AF}"/>
     <hyperlink ref="M10" r:id="rId9" xr:uid="{6E5CEB61-415E-4F8F-B8DA-C80BE1E50674}"/>
-    <hyperlink ref="S2" r:id="rId10" xr:uid="{30040BC6-F982-449E-AA51-9439DAD76E42}"/>
-    <hyperlink ref="S3" r:id="rId11" xr:uid="{FCCAF9C1-D8B8-4FB1-96BA-824DCB214589}"/>
-    <hyperlink ref="S4" r:id="rId12" xr:uid="{27C56937-0259-4A94-9386-F45108E6CC76}"/>
-    <hyperlink ref="S5" r:id="rId13" xr:uid="{087D66AF-CE27-4D1F-9B6A-BC2917E24E5E}"/>
-    <hyperlink ref="S6" r:id="rId14" xr:uid="{4212170C-2FCB-4117-A000-0D329FEC1D36}"/>
-    <hyperlink ref="S7" r:id="rId15" xr:uid="{E5AC18B6-B81A-43EC-8964-E60E80D53C28}"/>
-    <hyperlink ref="S8" r:id="rId16" xr:uid="{196A38F7-9B09-4D86-B03F-0689E41A6163}"/>
-    <hyperlink ref="S9" r:id="rId17" xr:uid="{49DAEEAF-5582-4FC3-886E-9F7847A59CEC}"/>
-    <hyperlink ref="S10" r:id="rId18" xr:uid="{C22DE3A3-7461-4171-AB93-2BD8C01E1780}"/>
-    <hyperlink ref="AJ2" r:id="rId19" xr:uid="{A5049F06-C56B-457A-9D79-B05FDFCF142D}"/>
-    <hyperlink ref="AJ3" r:id="rId20" xr:uid="{D67B98F9-BD3E-4484-A2CE-D98EED603587}"/>
-    <hyperlink ref="AJ4" r:id="rId21" xr:uid="{A2118C6E-4B18-4190-BB30-B541B9D9385A}"/>
-    <hyperlink ref="AJ5" r:id="rId22" xr:uid="{6BA3EFCB-64DE-4C69-A43C-724FA20D1AA1}"/>
-    <hyperlink ref="AJ6" r:id="rId23" xr:uid="{8E55B9FD-E2C9-4552-84F8-57F52ADB2F16}"/>
-    <hyperlink ref="AJ7" r:id="rId24" xr:uid="{33993A8D-97BE-4C0C-92CE-A5CE8D9F2B88}"/>
-    <hyperlink ref="AJ8" r:id="rId25" xr:uid="{2429D7B7-AE34-4978-A8AE-51ADB1624B78}"/>
-    <hyperlink ref="AJ9" r:id="rId26" xr:uid="{76754D97-F46F-437B-9C45-961A527E2839}"/>
-    <hyperlink ref="AJ10" r:id="rId27" xr:uid="{2C718935-29FB-4BD4-BD76-8CFAED7B3E72}"/>
-    <hyperlink ref="BI2" r:id="rId28" xr:uid="{9D83FFD7-180C-43A6-A8E7-16978F20FF6F}"/>
-    <hyperlink ref="BI3" r:id="rId29" xr:uid="{325F5191-3957-40D6-BF5F-B43932A62545}"/>
-    <hyperlink ref="BI4" r:id="rId30" xr:uid="{039D8190-BD56-4F0B-8B17-1D243EB543DA}"/>
-    <hyperlink ref="BI5" r:id="rId31" xr:uid="{76BEB2FF-4C46-47B4-AB3E-8EE133EC7DB6}"/>
-    <hyperlink ref="BI6" r:id="rId32" xr:uid="{BA61614A-A28B-4513-9BE6-22A8DCD29E83}"/>
-    <hyperlink ref="BI7" r:id="rId33" xr:uid="{D351EFCA-79AF-4A0F-ACBB-22D7BD7EA882}"/>
-    <hyperlink ref="BI8" r:id="rId34" xr:uid="{67895257-10B3-4B70-9790-54899BA795BB}"/>
-    <hyperlink ref="BI9" r:id="rId35" xr:uid="{760CB781-2359-4D70-A54B-B6898FEDAD45}"/>
-    <hyperlink ref="BI10" r:id="rId36" xr:uid="{5E22B85A-CF9A-4096-8BD1-F6A06E1A4F1A}"/>
+    <hyperlink ref="M11" r:id="rId10" xr:uid="{FF4C778A-B39E-480F-8C2D-24CD86C29C08}"/>
+    <hyperlink ref="S2" r:id="rId11" xr:uid="{F7AE5778-1156-4C88-B10E-28DDC74DF9E3}"/>
+    <hyperlink ref="S3" r:id="rId12" xr:uid="{C43C2B2F-F91A-4DDE-8AF9-2F9B807682E6}"/>
+    <hyperlink ref="S4" r:id="rId13" xr:uid="{3CD07D91-E449-4A08-B492-79A1D1D2F1DB}"/>
+    <hyperlink ref="S5" r:id="rId14" xr:uid="{F6A3EF43-429A-41F2-9045-4D6C75C8D7E2}"/>
+    <hyperlink ref="S6" r:id="rId15" xr:uid="{B339D9C9-6002-4DB9-A9E1-FB33C9BA862E}"/>
+    <hyperlink ref="S7" r:id="rId16" xr:uid="{2C91D6AA-0F93-4618-B0CB-6F7F1A8C6C2D}"/>
+    <hyperlink ref="S8" r:id="rId17" xr:uid="{FB70C968-76C4-459D-B466-7463B29073B3}"/>
+    <hyperlink ref="S9" r:id="rId18" xr:uid="{F656FACA-D930-44AD-AA73-75D4366A9877}"/>
+    <hyperlink ref="S10" r:id="rId19" xr:uid="{00268A6D-2348-45C0-93A1-D80E828E2AB9}"/>
+    <hyperlink ref="S11" r:id="rId20" xr:uid="{AA842F9D-6137-40ED-ABA0-9D35E1C69A93}"/>
+    <hyperlink ref="AJ2" r:id="rId21" xr:uid="{A77F8538-A387-4555-9BC1-143BD13364C2}"/>
+    <hyperlink ref="AJ3" r:id="rId22" xr:uid="{C4B2293C-EF15-4088-A910-5ACD2D952679}"/>
+    <hyperlink ref="AJ4" r:id="rId23" xr:uid="{64756216-8491-4EEF-8757-BCFB411EFD81}"/>
+    <hyperlink ref="AJ5" r:id="rId24" xr:uid="{C5475623-FD67-4340-B4D7-5B033E243995}"/>
+    <hyperlink ref="AJ6" r:id="rId25" xr:uid="{8DE0D65E-F95A-4796-AAC9-8261C7B46FF7}"/>
+    <hyperlink ref="AJ7" r:id="rId26" xr:uid="{BA7416C9-5282-4E8E-84C4-EAF10955D392}"/>
+    <hyperlink ref="AJ8" r:id="rId27" xr:uid="{13F80691-FA33-4803-9E42-E744E68AAF47}"/>
+    <hyperlink ref="AJ9" r:id="rId28" xr:uid="{D86E8EF4-CE7D-4471-8BD3-06DC1D3651A2}"/>
+    <hyperlink ref="AJ10" r:id="rId29" xr:uid="{6D29A8A4-6075-41CE-B918-45DD4111A189}"/>
+    <hyperlink ref="AJ11" r:id="rId30" xr:uid="{7175FC08-DBD9-48AF-B9FE-6ADFE356726E}"/>
+    <hyperlink ref="BI2" r:id="rId31" xr:uid="{F1B3D291-CC23-4735-9945-0C7C86DDA2F9}"/>
+    <hyperlink ref="BI3" r:id="rId32" xr:uid="{1C092722-81E6-49C2-BF0A-A20833F6429C}"/>
+    <hyperlink ref="BI4" r:id="rId33" xr:uid="{A67B821C-0461-4204-9BCD-B48A33FADA7B}"/>
+    <hyperlink ref="BI5" r:id="rId34" xr:uid="{878285B6-D697-4BE4-8DBA-4E084C616E47}"/>
+    <hyperlink ref="BI6" r:id="rId35" xr:uid="{F93F8755-9632-49A7-9FC2-94EB7C97FAB5}"/>
+    <hyperlink ref="BI7" r:id="rId36" xr:uid="{4E3594DF-3724-4FEF-A5C1-D5C7C539343E}"/>
+    <hyperlink ref="BI8" r:id="rId37" xr:uid="{DEA1222F-9728-4EC7-8044-E8F172679BB3}"/>
+    <hyperlink ref="BI9" r:id="rId38" xr:uid="{9D82FF9B-A4BB-4A9E-977B-EEC79C4A1B66}"/>
+    <hyperlink ref="BI10" r:id="rId39" xr:uid="{11BA9AFE-760E-4D8F-8E4A-CD0D881FF317}"/>
+    <hyperlink ref="BI11" r:id="rId40" xr:uid="{C18064E2-DFB7-44D3-8102-DFF434A98221}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregado test datos y ReqFun
</commit_message>
<xml_diff>
--- a/superAndes-jdo/data/DATOS.xlsx
+++ b/superAndes-jdo/data/DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Inc\Desktop\U\SisTrans\Iteracion 2\sistrans\superAndes-jdo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B361FB35-F0A8-40C7-8E55-D8390844A440}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1786D0D-B1E6-462D-AF1B-9535E0DD129C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{9796FEAD-349B-4125-A633-D95226379889}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="144">
   <si>
     <t>ID_ALMACENAMIENTO</t>
   </si>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E72C13-854D-4182-ADF2-AE51E01A9708}">
   <dimension ref="A1:CR18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0">
-      <selection activeCell="CG16" sqref="CG16"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,8 +1194,8 @@
       <c r="AL2">
         <v>1</v>
       </c>
-      <c r="AM2" t="s">
-        <v>97</v>
+      <c r="AM2">
+        <v>1</v>
       </c>
       <c r="AN2">
         <v>23</v>
@@ -1445,8 +1445,8 @@
       <c r="AL3">
         <v>2</v>
       </c>
-      <c r="AM3" t="s">
-        <v>98</v>
+      <c r="AM3">
+        <v>2</v>
       </c>
       <c r="AN3">
         <v>44</v>
@@ -1696,8 +1696,8 @@
       <c r="AL4">
         <v>3</v>
       </c>
-      <c r="AM4" t="s">
-        <v>99</v>
+      <c r="AM4">
+        <v>3</v>
       </c>
       <c r="AN4">
         <v>5</v>
@@ -1947,8 +1947,8 @@
       <c r="AL5">
         <v>4</v>
       </c>
-      <c r="AM5" t="s">
-        <v>97</v>
+      <c r="AM5">
+        <v>4</v>
       </c>
       <c r="AN5">
         <v>33</v>
@@ -2198,8 +2198,8 @@
       <c r="AL6">
         <v>5</v>
       </c>
-      <c r="AM6" t="s">
-        <v>97</v>
+      <c r="AM6">
+        <v>5</v>
       </c>
       <c r="AN6">
         <v>3</v>
@@ -2449,8 +2449,8 @@
       <c r="AL7">
         <v>6</v>
       </c>
-      <c r="AM7" t="s">
-        <v>100</v>
+      <c r="AM7">
+        <v>6</v>
       </c>
       <c r="AN7">
         <v>11</v>
@@ -2685,8 +2685,8 @@
       <c r="AL8">
         <v>7</v>
       </c>
-      <c r="AM8" t="s">
-        <v>100</v>
+      <c r="AM8">
+        <v>7</v>
       </c>
       <c r="AN8">
         <v>23</v>
@@ -2921,8 +2921,8 @@
       <c r="AL9">
         <v>8</v>
       </c>
-      <c r="AM9" t="s">
-        <v>101</v>
+      <c r="AM9">
+        <v>8</v>
       </c>
       <c r="AN9">
         <v>4</v>
@@ -3157,8 +3157,8 @@
       <c r="AL10">
         <v>9</v>
       </c>
-      <c r="AM10" t="s">
-        <v>102</v>
+      <c r="AM10">
+        <v>9</v>
       </c>
       <c r="AN10">
         <v>7</v>
@@ -3381,8 +3381,8 @@
       <c r="AL11">
         <v>10</v>
       </c>
-      <c r="AM11" t="s">
-        <v>103</v>
+      <c r="AM11">
+        <v>10</v>
       </c>
       <c r="AN11">
         <v>8</v>

</xml_diff>